<commit_message>
Se pueden editar y eliminar varias referencias del mismo pedido
Por ahora solo funciona si existen todas las referencias para esa orden
</commit_message>
<xml_diff>
--- a/AI_Engine/Resultados/Thyssenkrupp Campo Limpo/dataFrame.xlsx
+++ b/AI_Engine/Resultados/Thyssenkrupp Campo Limpo/dataFrame.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,7 +471,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C:\Users\IRDGFRM\Downloads\Prueba\thyssen_prueba.pdf</t>
+          <t>C:\Users\IRDGFRM\Downloads\20-04-2022_09h-22m.pdf</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>01.2022</t>
+          <t>08.2022</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -502,7 +502,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>C:\Users\IRDGFRM\Downloads\Prueba\thyssen_prueba.pdf</t>
+          <t>C:\Users\IRDGFRM\Downloads\20-04-2022_09h-22m.pdf</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -522,103 +522,10 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>08.2022</t>
+          <t>16.2022</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>C:\Users\IRDGFRM\Downloads\Prueba\thyssen_prueba.pdf</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>5500046535.</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>R544000</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>448</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>11.2022</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>C:\Users\IRDGFRM\Downloads\Prueba\thyssen_prueba.pdf</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>5500046535.</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>R544000</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>448</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>16.2022</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>C:\Users\IRDGFRM\Downloads\Prueba\thyssen_prueba.pdf</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>5500046535.</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>R544000</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>448</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>20.2022</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>